<commit_message>
dokumentaatio paivitys ja koodin siivous
</commit_message>
<xml_diff>
--- a/Dokumentaatio/suoritukykytulokset.xlsx
+++ b/Dokumentaatio/suoritukykytulokset.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Koulujuttuja\tiralabra\Dokumentaatio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Koulujuttuja\tiralabra\dokumentaatio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DE6B77-96E6-4598-A1CF-387F48142FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E28E6A87-6298-460A-934B-53E62D97A5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{61AB70EE-FA37-4313-A6B8-EFB47798ABB0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{61AB70EE-FA37-4313-A6B8-EFB47798ABB0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Taul1" sheetId="1" r:id="rId1"/>
+    <sheet name="Taul1 (2)" sheetId="3" r:id="rId1"/>
+    <sheet name="Taul1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="6">
   <si>
     <t>syvyys</t>
   </si>
@@ -93,7 +95,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -111,7 +113,866 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fi-FI"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Taul1 (2)'!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>asemat</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-FI"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Taul1 (2)'!$C$4:$D$12</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="9"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>On</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>On</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>On</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>On</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>On</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Ei</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Ei</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Ei</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>4</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Taul1 (2)'!$F$4:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3441</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9582</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>280603</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>677792</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>925</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30271</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1044789</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A9B4-4075-BDF8-60AFA4D0985B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="269"/>
+        <c:axId val="308360128"/>
+        <c:axId val="1298221888"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Taul1 (2)'!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>aika</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-FI"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Taul1 (2)'!$C$4:$D$12</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="9"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>On</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>On</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>On</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>On</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>On</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Ei</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Ei</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Ei</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>4</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Taul1 (2)'!$E$4:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6.6000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5269999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5190000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>110.093</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>243.01599999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.441</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.253</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>462.93299999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A9B4-4075-BDF8-60AFA4D0985B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="308349568"/>
+        <c:axId val="1298222384"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="308360128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-FI"/>
+                  <a:t>Syvyys</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-FI" baseline="0"/>
+                  <a:t> ja alphabeetta-karsinta on/ei</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-FI"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-FI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1298221888"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1298221888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-FI"/>
+                  <a:t>Läpikäytyjen</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-FI" baseline="0"/>
+                  <a:t> asemien määrä</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-FI"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-FI"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-FI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="308360128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1298222384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-FI"/>
+                  <a:t>Aika (Sekuntteina)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-FI"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-FI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="308349568"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="308349568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1298222384"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-FI"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-FI"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1037,6 +1898,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="225">
   <cs:axisTitle>
@@ -1537,7 +2438,550 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="225">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="2000" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Kaavio 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC6CAB09-3609-4052-A075-70ADB2EF4B17}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1579,9 +3023,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-teema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1619,7 +3063,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1725,7 +3169,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1867,18 +3311,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B98A61-9597-47F2-9745-CFC14C017CDE}">
-  <dimension ref="C3:F14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBBDABF0-9C26-42D7-A1A4-945E564B78A7}">
+  <dimension ref="C3:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U29" sqref="U29"/>
+      <selection activeCell="Y15" sqref="Y15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1905,10 +3349,10 @@
         <v>4</v>
       </c>
       <c r="E4">
-        <v>0.2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="F4">
-        <v>304</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.25">
@@ -1919,10 +3363,10 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <v>0.9</v>
+        <v>1.5269999999999999</v>
       </c>
       <c r="F5">
-        <v>1594</v>
+        <v>3441</v>
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
@@ -1933,10 +3377,10 @@
         <v>4</v>
       </c>
       <c r="E6">
-        <v>12</v>
+        <v>3.5190000000000001</v>
       </c>
       <c r="F6">
-        <v>22757</v>
+        <v>9582</v>
       </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.25">
@@ -1947,10 +3391,10 @@
         <v>4</v>
       </c>
       <c r="E7">
-        <v>41</v>
+        <v>110.093</v>
       </c>
       <c r="F7">
-        <v>86495</v>
+        <v>280603</v>
       </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
@@ -1961,10 +3405,10 @@
         <v>4</v>
       </c>
       <c r="E8">
-        <v>803</v>
+        <v>243.01599999999999</v>
       </c>
       <c r="F8">
-        <v>1498344</v>
+        <v>677792</v>
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
@@ -1975,10 +3419,10 @@
         <v>5</v>
       </c>
       <c r="E10">
-        <v>0.2</v>
+        <v>0.441</v>
       </c>
       <c r="F10">
-        <v>304</v>
+        <v>925</v>
       </c>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.25">
@@ -1989,10 +3433,10 @@
         <v>5</v>
       </c>
       <c r="E11">
-        <v>4</v>
+        <v>13.253</v>
       </c>
       <c r="F11">
-        <v>6896</v>
+        <v>30271</v>
       </c>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.25">
@@ -2003,32 +3447,10 @@
         <v>5</v>
       </c>
       <c r="E12">
-        <v>101</v>
+        <v>462.93299999999999</v>
       </c>
       <c r="F12">
-        <v>166136</v>
-      </c>
-    </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C13">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13">
-        <v>2540</v>
-      </c>
-      <c r="F13">
-        <v>4383320</v>
-      </c>
-    </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C14">
-        <v>6</v>
-      </c>
-      <c r="D14" t="s">
-        <v>5</v>
+        <v>1044789</v>
       </c>
     </row>
   </sheetData>
@@ -2036,4 +3458,181 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B98A61-9597-47F2-9745-CFC14C017CDE}">
+  <dimension ref="C3:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>0.2</v>
+      </c>
+      <c r="F4">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>0.9</v>
+      </c>
+      <c r="F5">
+        <v>1594</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>12</v>
+      </c>
+      <c r="F6">
+        <v>22757</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>41</v>
+      </c>
+      <c r="F7">
+        <v>86495</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>803</v>
+      </c>
+      <c r="F8">
+        <v>1498344</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>0.2</v>
+      </c>
+      <c r="F10">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <v>6896</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>101</v>
+      </c>
+      <c r="F12">
+        <v>166136</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>2540</v>
+      </c>
+      <c r="F13">
+        <v>4383320</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1661C9C-88C5-4840-812E-4F910BB573B2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>